<commit_message>
Update 2020-12-04 BROObject - GAR IMBRO data exchange file (v0.99).xlsx
</commit_message>
<xml_diff>
--- a/2020-12-04 BROObject - GAR IMBRO data exchange file (v0.99).xlsx
+++ b/2020-12-04 BROObject - GAR IMBRO data exchange file (v0.99).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/Projecten/20107A - BZK - Excel format BRO objecten/Formats/GAR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{158E896A-FE3B-4C77-B4A1-A4191A45AA21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9858066F-27EA-4D47-9FE4-3D3791B6CC01}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{158E896A-FE3B-4C77-B4A1-A4191A45AA21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E57D4920-93F1-401C-BB3F-97360983D429}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="679" xr2:uid="{26814B37-6F38-4D5A-99CF-A0A5CD7480CB}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5468" uniqueCount="2996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5469" uniqueCount="2997">
   <si>
     <t>Format Name</t>
   </si>
@@ -9042,6 +9042,9 @@
   </si>
   <si>
     <t>FieldVisit</t>
+  </si>
+  <si>
+    <t>GAR</t>
   </si>
 </sst>
 </file>
@@ -10110,7 +10113,9 @@
       <c r="A11" s="24">
         <v>1</v>
       </c>
-      <c r="B11" s="27"/>
+      <c r="B11" s="27" t="s">
+        <v>2996</v>
+      </c>
       <c r="C11" s="15" t="s">
         <v>2991</v>
       </c>

</xml_diff>